<commit_message>
subscription and shipment pages
woohoo :-)
</commit_message>
<xml_diff>
--- a/db/gums seed data v4.xlsx
+++ b/db/gums seed data v4.xlsx
@@ -902,7 +902,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="608">
+  <cellStyleXfs count="626">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1511,8 +1511,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1541,8 +1559,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="475" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="608">
+  <cellStyles count="626">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1912,6 +1933,24 @@
     <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2482,8 +2521,8 @@
   <dimension ref="A1:K189"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G118" sqref="G118"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3713,7 +3752,7 @@
       <c r="E34" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="9" t="s">
         <v>171</v>
       </c>
       <c r="G34" s="6" t="s">
@@ -3750,7 +3789,7 @@
       <c r="E35" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G35" s="6" t="s">
@@ -3787,7 +3826,7 @@
       <c r="E36" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G36" s="6" t="s">
@@ -3824,7 +3863,7 @@
       <c r="E37" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G37" s="6" t="s">
@@ -3861,7 +3900,7 @@
       <c r="E38" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G38" s="6" t="s">
@@ -3898,7 +3937,7 @@
       <c r="E39" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G39" s="6" t="s">
@@ -3935,7 +3974,7 @@
       <c r="E40" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G40" s="6" t="s">
@@ -3972,7 +4011,7 @@
       <c r="E41" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="9" t="s">
         <v>36</v>
       </c>
       <c r="G41" s="6" t="s">
@@ -4009,7 +4048,7 @@
       <c r="E42" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="9" t="s">
         <v>37</v>
       </c>
       <c r="G42" s="6" t="s">
@@ -4063,36 +4102,36 @@
         <v>dentyne_ice_peppermint.png</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="4" t="str">
+    <row r="44" spans="1:11" s="9" customFormat="1">
+      <c r="A44" s="9" t="str">
         <f t="shared" si="0"/>
         <v>dentyne_ice_spearmint</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="C44" s="4">
-        <v>1</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="B44" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="G44" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="J44" s="4">
-        <v>0</v>
-      </c>
-      <c r="K44" s="4" t="str">
+      <c r="I44" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J44" s="9">
+        <v>0</v>
+      </c>
+      <c r="K44" s="9" t="str">
         <f t="shared" si="13"/>
         <v>dentyne_ice_spearmint.png</v>
       </c>
@@ -5903,6 +5942,10 @@
       <c r="J97" s="4">
         <v>0</v>
       </c>
+      <c r="K97" s="4" t="str">
+        <f t="shared" ref="K97:K108" si="29">CONCATENATE(A97,".jpg")</f>
+        <v>5_gum_rain.jpg</v>
+      </c>
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="4" t="str">
@@ -5933,6 +5976,10 @@
       <c r="J98" s="4">
         <v>0</v>
       </c>
+      <c r="K98" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_cobalt.jpg</v>
+      </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" s="4" t="str">
@@ -5963,6 +6010,10 @@
       <c r="J99" s="4">
         <v>0</v>
       </c>
+      <c r="K99" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_flare.jpg</v>
+      </c>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="9" t="str">
@@ -5993,6 +6044,10 @@
       <c r="J100" s="4">
         <v>0</v>
       </c>
+      <c r="K100" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_elixir.jpg</v>
+      </c>
     </row>
     <row r="101" spans="1:11">
       <c r="A101" s="9" t="str">
@@ -6023,6 +6078,10 @@
       <c r="J101" s="4">
         <v>0</v>
       </c>
+      <c r="K101" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_solstice.jpg</v>
+      </c>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="9" t="str">
@@ -6053,6 +6112,10 @@
       <c r="J102" s="4">
         <v>0</v>
       </c>
+      <c r="K102" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_react_fruit.jpg</v>
+      </c>
     </row>
     <row r="103" spans="1:11">
       <c r="A103" s="9" t="str">
@@ -6083,6 +6146,10 @@
       <c r="J103" s="4">
         <v>0</v>
       </c>
+      <c r="K103" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_react_mint.jpg</v>
+      </c>
     </row>
     <row r="104" spans="1:11">
       <c r="A104" s="9" t="str">
@@ -6113,6 +6180,10 @@
       <c r="J104" s="4">
         <v>0</v>
       </c>
+      <c r="K104" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_prism.jpg</v>
+      </c>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="9" t="str">
@@ -6143,6 +6214,10 @@
       <c r="J105" s="4">
         <v>0</v>
       </c>
+      <c r="K105" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_vortex.jpg</v>
+      </c>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="9" t="str">
@@ -6173,6 +6248,10 @@
       <c r="J106" s="4">
         <v>0</v>
       </c>
+      <c r="K106" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_swerve.jpg</v>
+      </c>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="9" t="str">
@@ -6203,6 +6282,10 @@
       <c r="J107" s="4">
         <v>0</v>
       </c>
+      <c r="K107" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_rpm_fruit.jpg</v>
+      </c>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="9" t="str">
@@ -6233,6 +6316,10 @@
       <c r="J108" s="4">
         <v>0</v>
       </c>
+      <c r="K108" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>5_gum_rpm_mint.jpg</v>
+      </c>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" s="4" t="str">
@@ -6298,7 +6385,7 @@
         <v>0</v>
       </c>
       <c r="K110" s="4" t="str">
-        <f t="shared" ref="K110:K117" si="29">CONCATENATE(A110,".jpg")</f>
+        <f t="shared" ref="K110:K117" si="30">CONCATENATE(A110,".jpg")</f>
         <v>wrigleys_doublemint_mint.jpg</v>
       </c>
     </row>
@@ -6332,7 +6419,7 @@
         <v>0</v>
       </c>
       <c r="K111" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>eclipse_spearmint.jpg</v>
       </c>
     </row>
@@ -6366,7 +6453,7 @@
         <v>0</v>
       </c>
       <c r="K112" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>eclipse_polar_ice.jpg</v>
       </c>
     </row>
@@ -6400,7 +6487,7 @@
         <v>0</v>
       </c>
       <c r="K113" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>eclipse_peppermint.jpg</v>
       </c>
     </row>
@@ -6434,7 +6521,7 @@
         <v>0</v>
       </c>
       <c r="K114" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>eclipse_winterfrost.jpg</v>
       </c>
     </row>
@@ -6468,7 +6555,7 @@
         <v>0</v>
       </c>
       <c r="K115" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>freedent_peppermint.jpg</v>
       </c>
     </row>
@@ -6502,7 +6589,7 @@
         <v>0</v>
       </c>
       <c r="K116" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>freedent_spearmint.jpg</v>
       </c>
     </row>
@@ -6536,7 +6623,7 @@
         <v>0</v>
       </c>
       <c r="K117" s="4" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>freedent_winterfresh.jpg</v>
       </c>
     </row>
@@ -7460,7 +7547,7 @@
     </row>
     <row r="152" spans="1:10">
       <c r="A152" s="4" t="str">
-        <f t="shared" ref="A152:A155" si="30">SUBSTITUTE(LOWER(CONCATENATE(SUBSTITUTE(E152," ","_"),"_",SUBSTITUTE(F152," ","_"))),"'","")</f>
+        <f t="shared" ref="A152:A155" si="31">SUBSTITUTE(LOWER(CONCATENATE(SUBSTITUTE(E152," ","_"),"_",SUBSTITUTE(F152," ","_"))),"'","")</f>
         <v>orbit_white_peppermint</v>
       </c>
       <c r="B152" s="7" t="s">
@@ -7487,7 +7574,7 @@
     </row>
     <row r="153" spans="1:10">
       <c r="A153" s="4" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>orbit_white_spearmint</v>
       </c>
       <c r="B153" s="7" t="s">
@@ -7514,7 +7601,7 @@
     </row>
     <row r="154" spans="1:10">
       <c r="A154" s="4" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>wrigleys_winterfresh</v>
       </c>
       <c r="B154" s="7" t="s">
@@ -7541,7 +7628,7 @@
     </row>
     <row r="155" spans="1:10">
       <c r="A155" s="4" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>wrigleys_spearmint</v>
       </c>
       <c r="B155" s="7" t="s">
@@ -8001,7 +8088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A133"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:A95"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -8304,20 +8393,20 @@
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="str">
-        <f>CONCATENATE(Sheet1!A67,"|",Sheet1!B67,"|",Sheet1!C67,"|",Sheet1!D67,"|",Sheet1!E67,"|",Sheet1!F67,"|",Sheet1!G67,"|",Sheet1!H67,"|",Sheet1!I67,"|",Sheet1!J67,"|",Sheet1!K67)</f>
-        <v>stride_whitemint|0|1|Kraft Foods Cadburry|Stride|Whitemint|?||United States|0|stride_whitemint.jpg</v>
+        <f>CONCATENATE(Sheet1!A51,"|",Sheet1!B51,"|",Sheet1!C51,"|",Sheet1!D51,"|",Sheet1!E51,"|",Sheet1!F51,"|",Sheet1!G51,"|",Sheet1!H51,"|",Sheet1!I51,"|",Sheet1!J51,"|",Sheet1!K51)</f>
+        <v>stride_spark_kinetic_fruit|0|1|Kraft Foods Cadburry|Stride Spark|Kinetic Fruit|?||United States|0|stride_spark_kinetic_fruit.jpg</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="str">
-        <f>CONCATENATE(Sheet1!A51,"|",Sheet1!B51,"|",Sheet1!C51,"|",Sheet1!D51,"|",Sheet1!E51,"|",Sheet1!F51,"|",Sheet1!G51,"|",Sheet1!H51,"|",Sheet1!I51,"|",Sheet1!J51,"|",Sheet1!K51)</f>
-        <v>stride_spark_kinetic_fruit|0|1|Kraft Foods Cadburry|Stride Spark|Kinetic Fruit|?||United States|0|stride_spark_kinetic_fruit.jpg</v>
+        <f>CONCATENATE(Sheet1!A52,"|",Sheet1!B52,"|",Sheet1!C52,"|",Sheet1!D52,"|",Sheet1!E52,"|",Sheet1!F52,"|",Sheet1!G52,"|",Sheet1!H52,"|",Sheet1!I52,"|",Sheet1!J52,"|",Sheet1!K52)</f>
+        <v>stride_spark_kinetic_mint|0|1|Kraft Foods Cadburry|Stride Spark|Kinetic Mint|?||United States|0|stride_spark_kinetic_mint.jpg</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="str">
-        <f>CONCATENATE(Sheet1!A52,"|",Sheet1!B52,"|",Sheet1!C52,"|",Sheet1!D52,"|",Sheet1!E52,"|",Sheet1!F52,"|",Sheet1!G52,"|",Sheet1!H52,"|",Sheet1!I52,"|",Sheet1!J52,"|",Sheet1!K52)</f>
-        <v>stride_spark_kinetic_mint|0|1|Kraft Foods Cadburry|Stride Spark|Kinetic Mint|?||United States|0|stride_spark_kinetic_mint.jpg</v>
+        <f>CONCATENATE(Sheet1!A53,"|",Sheet1!B53,"|",Sheet1!C53,"|",Sheet1!D53,"|",Sheet1!E53,"|",Sheet1!F53,"|",Sheet1!G53,"|",Sheet1!H53,"|",Sheet1!I53,"|",Sheet1!J53,"|",Sheet1!K53)</f>
+        <v>stride_spark_kinetic_berry|0|1|Kraft Foods Cadburry|Stride Spark|Kinetic Berry|?||United States|0|stride_spark_kinetic_berry.jpg</v>
       </c>
     </row>
     <row r="53" spans="1:1">
@@ -8364,446 +8453,446 @@
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="str">
+        <f>CONCATENATE(Sheet1!A61,"|",Sheet1!B61,"|",Sheet1!C61,"|",Sheet1!D61,"|",Sheet1!E61,"|",Sheet1!F61,"|",Sheet1!G61,"|",Sheet1!H61,"|",Sheet1!I61,"|",Sheet1!J61,"|",Sheet1!K61)</f>
+        <v>stride_2.0_sweet_mint|0|1|Kraft Foods Cadburry|Stride 2.0|Sweet Mint|?||United States|0|stride_2.0_sweet_mint.jpg</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="str">
         <f>CONCATENATE(Sheet1!A62,"|",Sheet1!B62,"|",Sheet1!C62,"|",Sheet1!D62,"|",Sheet1!E62,"|",Sheet1!F62,"|",Sheet1!G62,"|",Sheet1!H62,"|",Sheet1!I62,"|",Sheet1!J62,"|",Sheet1!K62)</f>
         <v>stride_2.0_spearmint|0|1|Kraft Foods Cadburry|Stride 2.0|Spearmint|?||United States|0|stride_2.0_spearmint.jpg</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="str">
+    <row r="62" spans="1:1">
+      <c r="A62" t="str">
         <f>CONCATENATE(Sheet1!A63,"|",Sheet1!B63,"|",Sheet1!C63,"|",Sheet1!D63,"|",Sheet1!E63,"|",Sheet1!F63,"|",Sheet1!G63,"|",Sheet1!H63,"|",Sheet1!I63,"|",Sheet1!J63,"|",Sheet1!K63)</f>
         <v>stride_2.0_nonstop_mint|0|1|Kraft Foods Cadburry|Stride 2.0|Nonstop Mint|?||United States|0|stride_2.0_nonstop_mint.jpg</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="str">
+    <row r="63" spans="1:1">
+      <c r="A63" t="str">
         <f>CONCATENATE(Sheet1!A64,"|",Sheet1!B64,"|",Sheet1!C64,"|",Sheet1!D64,"|",Sheet1!E64,"|",Sheet1!F64,"|",Sheet1!G64,"|",Sheet1!H64,"|",Sheet1!I64,"|",Sheet1!J64,"|",Sheet1!K64)</f>
         <v>stride_2.0_forever_fruit|0|1|Kraft Foods Cadburry|Stride 2.0|Forever Fruit|?||United States|0|stride_2.0_forever_fruit.jpg</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="str">
+    <row r="64" spans="1:1">
+      <c r="A64" t="str">
+        <f>CONCATENATE(Sheet1!A65,"|",Sheet1!B65,"|",Sheet1!C65,"|",Sheet1!D65,"|",Sheet1!E65,"|",Sheet1!F65,"|",Sheet1!G65,"|",Sheet1!H65,"|",Sheet1!I65,"|",Sheet1!J65,"|",Sheet1!K65)</f>
+        <v>stride_mintacular|0|1|Kraft Foods Cadburry|Stride|Mintacular|?||United States|0|stride_mintacular.jpg</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="str">
         <f>CONCATENATE(Sheet1!A66,"|",Sheet1!B66,"|",Sheet1!C66,"|",Sheet1!D66,"|",Sheet1!E66,"|",Sheet1!F66,"|",Sheet1!G66,"|",Sheet1!H66,"|",Sheet1!I66,"|",Sheet1!J66,"|",Sheet1!K66)</f>
         <v>stride_mega_mystery|0|1|Kraft Foods Cadburry|Stride|Mega Mystery|?||United States|0|stride_mega_mystery.jpg</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="str">
+    <row r="66" spans="1:1">
+      <c r="A66" t="str">
+        <f>CONCATENATE(Sheet1!A67,"|",Sheet1!B67,"|",Sheet1!C67,"|",Sheet1!D67,"|",Sheet1!E67,"|",Sheet1!F67,"|",Sheet1!G67,"|",Sheet1!H67,"|",Sheet1!I67,"|",Sheet1!J67,"|",Sheet1!K67)</f>
+        <v>stride_whitemint|0|1|Kraft Foods Cadburry|Stride|Whitemint|?||United States|0|stride_whitemint.jpg</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="str">
+        <f>CONCATENATE(Sheet1!A68,"|",Sheet1!B68,"|",Sheet1!C68,"|",Sheet1!D68,"|",Sheet1!E68,"|",Sheet1!F68,"|",Sheet1!G68,"|",Sheet1!H68,"|",Sheet1!I68,"|",Sheet1!J68,"|",Sheet1!K68)</f>
+        <v>stride_tropical_trance|0|1|Kraft Foods Cadburry|Stride|Tropical Trance|?||United States|0|stride_tropical_trance.jpg</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="str">
+        <f>CONCATENATE(Sheet1!A69,"|",Sheet1!B69,"|",Sheet1!C69,"|",Sheet1!D69,"|",Sheet1!E69,"|",Sheet1!F69,"|",Sheet1!G69,"|",Sheet1!H69,"|",Sheet1!I69,"|",Sheet1!J69,"|",Sheet1!K69)</f>
+        <v>stride_eternal_melon|0|1|Kraft Foods Cadburry|Stride|Eternal Melon|?||United States|0|stride_eternal_melon.jpg</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="str">
+        <f>CONCATENATE(Sheet1!A70,"|",Sheet1!B70,"|",Sheet1!C70,"|",Sheet1!D70,"|",Sheet1!E70,"|",Sheet1!F70,"|",Sheet1!G70,"|",Sheet1!H70,"|",Sheet1!I70,"|",Sheet1!J70,"|",Sheet1!K70)</f>
+        <v>stride_nonstop_mint|0|0|Kraft Foods Cadburry|Stride|Nonstop Mint|?||United States|0|stride_nonstop_mint.jpg</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="str">
+        <f>CONCATENATE(Sheet1!A71,"|",Sheet1!B71,"|",Sheet1!C71,"|",Sheet1!D71,"|",Sheet1!E71,"|",Sheet1!F71,"|",Sheet1!G71,"|",Sheet1!H71,"|",Sheet1!I71,"|",Sheet1!J71,"|",Sheet1!K71)</f>
+        <v>stride_winterblue|0|0|Kraft Foods Cadburry|Stride|Winterblue|?||United States|0|stride_winterblue.jpg</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="str">
+        <f>CONCATENATE(Sheet1!A72,"|",Sheet1!B72,"|",Sheet1!C72,"|",Sheet1!D72,"|",Sheet1!E72,"|",Sheet1!F72,"|",Sheet1!G72,"|",Sheet1!H72,"|",Sheet1!I72,"|",Sheet1!J72,"|",Sheet1!K72)</f>
+        <v>stride_spearmint|0|0|Kraft Foods Cadburry|Stride|Spearmint|?||United States|0|stride_spearmint.jpg</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="str">
+        <f>CONCATENATE(Sheet1!A73,"|",Sheet1!B73,"|",Sheet1!C73,"|",Sheet1!D73,"|",Sheet1!E73,"|",Sheet1!F73,"|",Sheet1!G73,"|",Sheet1!H73,"|",Sheet1!I73,"|",Sheet1!J73,"|",Sheet1!K73)</f>
+        <v>stride_sweet_peppermint|0|0|Kraft Foods Cadburry|Stride|Sweet Peppermint|?||United States|0|stride_sweet_peppermint.jpg</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="str">
+        <f>CONCATENATE(Sheet1!A74,"|",Sheet1!B74,"|",Sheet1!C74,"|",Sheet1!D74,"|",Sheet1!E74,"|",Sheet1!F74,"|",Sheet1!G74,"|",Sheet1!H74,"|",Sheet1!I74,"|",Sheet1!J74,"|",Sheet1!K74)</f>
+        <v>stride_sweet_berry|0|0|Kraft Foods Cadburry|Stride|Sweet Berry|?||United States|0|stride_sweet_berry.jpg</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="str">
+        <f>CONCATENATE(Sheet1!A75,"|",Sheet1!B75,"|",Sheet1!C75,"|",Sheet1!D75,"|",Sheet1!E75,"|",Sheet1!F75,"|",Sheet1!G75,"|",Sheet1!H75,"|",Sheet1!I75,"|",Sheet1!J75,"|",Sheet1!K75)</f>
+        <v>stride_uber_bubble|0|0|Kraft Foods Cadburry|Stride|Uber Bubble|?||United States|0|stride_uber_bubble.jpg</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="str">
+        <f>CONCATENATE(Sheet1!A76,"|",Sheet1!B76,"|",Sheet1!C76,"|",Sheet1!D76,"|",Sheet1!E76,"|",Sheet1!F76,"|",Sheet1!G76,"|",Sheet1!H76,"|",Sheet1!I76,"|",Sheet1!J76,"|",Sheet1!K76)</f>
+        <v>stride_sweet_cinnamon|0|0|Kraft Foods Cadburry|Stride|Sweet Cinnamon|?||United States|0|stride_sweet_cinnamon.jpg</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="str">
+        <f>CONCATENATE(Sheet1!A77,"|",Sheet1!B77,"|",Sheet1!C77,"|",Sheet1!D77,"|",Sheet1!E77,"|",Sheet1!F77,"|",Sheet1!G77,"|",Sheet1!H77,"|",Sheet1!I77,"|",Sheet1!J77,"|",Sheet1!K77)</f>
+        <v>stride_forever_fruit|0|0|Kraft Foods Cadburry|Stride|Forever Fruit|?||United States|0|stride_forever_fruit.jpg</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="str">
+        <f>CONCATENATE(Sheet1!A78,"|",Sheet1!B78,"|",Sheet1!C78,"|",Sheet1!D78,"|",Sheet1!E78,"|",Sheet1!F78,"|",Sheet1!G78,"|",Sheet1!H78,"|",Sheet1!I78,"|",Sheet1!J78,"|",Sheet1!K78)</f>
+        <v>stride_always_mandarin|0|1|Kraft Foods Cadburry|Stride|Always Mandarin|?||United States|0|stride_always_mandarin.jpg</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="str">
         <f>CONCATENATE(Sheet1!A79,"|",Sheet1!B79,"|",Sheet1!C79,"|",Sheet1!D79,"|",Sheet1!E79,"|",Sheet1!F79,"|",Sheet1!G79,"|",Sheet1!H79,"|",Sheet1!I79,"|",Sheet1!J79,"|",Sheet1!K79)</f>
         <v>adams_chiclets_fruit|0|1|Kraft Foods Cadburry|Adam's Chiclets|fruit|?||United States|0|adams_chiclets_fruit.jpg</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="e">
-        <f>CONCATENATE(Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!,"|",Sheet1!#REF!)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="str">
+    <row r="79" spans="1:1">
+      <c r="A79" t="str">
         <f>CONCATENATE(Sheet1!A80,"|",Sheet1!B80,"|",Sheet1!C80,"|",Sheet1!D80,"|",Sheet1!E80,"|",Sheet1!F80,"|",Sheet1!G80,"|",Sheet1!H80,"|",Sheet1!I80,"|",Sheet1!J80,"|",Sheet1!K80)</f>
         <v>adams_chiclets_peppermint|0|1|Kraft Foods Cadburry|Adam's Chiclets|peppermint|?||United States|0|adams_chiclets_peppermint.jpg</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="str">
+    <row r="80" spans="1:1">
+      <c r="A80" t="str">
         <f>CONCATENATE(Sheet1!A81,"|",Sheet1!B81,"|",Sheet1!C81,"|",Sheet1!D81,"|",Sheet1!E81,"|",Sheet1!F81,"|",Sheet1!G81,"|",Sheet1!H81,"|",Sheet1!I81,"|",Sheet1!J81,"|",Sheet1!K81)</f>
         <v>adams_chiclets_spearmint|0|1|Kraft Foods Cadburry|Adam's Chiclets|spearmint|?||United States|0|adams_chiclets_spearmint.jpg</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="str">
+    <row r="81" spans="1:1">
+      <c r="A81" t="str">
         <f>CONCATENATE(Sheet1!A82,"|",Sheet1!B82,"|",Sheet1!C82,"|",Sheet1!D82,"|",Sheet1!E82,"|",Sheet1!F82,"|",Sheet1!G82,"|",Sheet1!H82,"|",Sheet1!I82,"|",Sheet1!J82,"|",Sheet1!K82)</f>
         <v>extra_dessert_delights_apple_pie|022000013835|1|Mars Inc Wrigley|Extra Dessert Delights|Apple Pie|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_dessert_delights_apple_pie.png</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="str">
+    <row r="82" spans="1:1">
+      <c r="A82" t="str">
         <f>CONCATENATE(Sheet1!A83,"|",Sheet1!B83,"|",Sheet1!C83,"|",Sheet1!D83,"|",Sheet1!E83,"|",Sheet1!F83,"|",Sheet1!G83,"|",Sheet1!H83,"|",Sheet1!I83,"|",Sheet1!J83,"|",Sheet1!K83)</f>
         <v>extra_dessert_delights_orange_creme_pop|022000013187|1|Mars Inc Wrigley|Extra Dessert Delights|Orange Creme Pop|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_dessert_delights_orange_creme_pop.png</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="str">
+    <row r="83" spans="1:1">
+      <c r="A83" t="str">
         <f>CONCATENATE(Sheet1!A84,"|",Sheet1!B84,"|",Sheet1!C84,"|",Sheet1!D84,"|",Sheet1!E84,"|",Sheet1!F84,"|",Sheet1!G84,"|",Sheet1!H84,"|",Sheet1!I84,"|",Sheet1!J84,"|",Sheet1!K84)</f>
         <v>extra_dessert_delights_mint_chocolate_chip|022000115638|1|Mars Inc Wrigley|Extra Dessert Delights|Mint Chocolate Chip|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_dessert_delights_mint_chocolate_chip.png</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="str">
+    <row r="84" spans="1:1">
+      <c r="A84" t="str">
         <f>CONCATENATE(Sheet1!A85,"|",Sheet1!B85,"|",Sheet1!C85,"|",Sheet1!D85,"|",Sheet1!E85,"|",Sheet1!F85,"|",Sheet1!G85,"|",Sheet1!H85,"|",Sheet1!I85,"|",Sheet1!J85,"|",Sheet1!K85)</f>
         <v>extra_dessert_delights_strawberry_shortcake|0|1|Mars Inc Wrigley|Extra Dessert Delights|Strawberry Shortcake|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_dessert_delights_strawberry_shortcake.png</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="str">
+    <row r="85" spans="1:1">
+      <c r="A85" t="str">
         <f>CONCATENATE(Sheet1!A86,"|",Sheet1!B86,"|",Sheet1!C86,"|",Sheet1!D86,"|",Sheet1!E86,"|",Sheet1!F86,"|",Sheet1!G86,"|",Sheet1!H86,"|",Sheet1!I86,"|",Sheet1!J86,"|",Sheet1!K86)</f>
         <v>extra_dessert_delights_key_lime_pie|022000115621|1|Mars Inc Wrigley|Extra Dessert Delights|Key Lime Pie|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_dessert_delights_key_lime_pie.png</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="str">
+    <row r="86" spans="1:1">
+      <c r="A86" t="str">
+        <f>CONCATENATE(Sheet1!A87,"|",Sheet1!B87,"|",Sheet1!C87,"|",Sheet1!D87,"|",Sheet1!E87,"|",Sheet1!F87,"|",Sheet1!G87,"|",Sheet1!H87,"|",Sheet1!I87,"|",Sheet1!J87,"|",Sheet1!K87)</f>
+        <v>extra_dessert_delights_root_beer_float|0|1|Mars Inc Wrigley|Extra Dessert Delights|Root Beer Float|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_dessert_delights_root_beer_float.png</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="str">
+        <f>CONCATENATE(Sheet1!A88,"|",Sheet1!B88,"|",Sheet1!C88,"|",Sheet1!D88,"|",Sheet1!E88,"|",Sheet1!F88,"|",Sheet1!G88,"|",Sheet1!H88,"|",Sheet1!I88,"|",Sheet1!J88,"|",Sheet1!K88)</f>
+        <v>extra_dessert_delights_rainbow_sherbert|0|1|Mars Inc Wrigley|Extra Dessert Delights|Rainbow Sherbert|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_dessert_delights_rainbow_sherbert.png</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="str">
         <f>CONCATENATE(Sheet1!A89,"|",Sheet1!B89,"|",Sheet1!C89,"|",Sheet1!D89,"|",Sheet1!E89,"|",Sheet1!F89,"|",Sheet1!G89,"|",Sheet1!H89,"|",Sheet1!I89,"|",Sheet1!J89,"|",Sheet1!K89)</f>
         <v>extra_fruit_sensations_sweet_watermelon|0|1|Mars Inc Wrigley|Extra Fruit Sensations|Sweet Watermelon|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_fruit_sensations_sweet_watermelon.png</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="str">
+    <row r="89" spans="1:1">
+      <c r="A89" t="str">
         <f>CONCATENATE(Sheet1!A90,"|",Sheet1!B90,"|",Sheet1!C90,"|",Sheet1!D90,"|",Sheet1!E90,"|",Sheet1!F90,"|",Sheet1!G90,"|",Sheet1!H90,"|",Sheet1!I90,"|",Sheet1!J90,"|",Sheet1!K90)</f>
         <v>extra_fruit_sensations_sweet_tropical|0|1|Mars Inc Wrigley|Extra Fruit Sensations|Sweet Tropical|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_fruit_sensations_sweet_tropical.png</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="str">
+    <row r="90" spans="1:1">
+      <c r="A90" t="str">
         <f>CONCATENATE(Sheet1!A91,"|",Sheet1!B91,"|",Sheet1!C91,"|",Sheet1!D91,"|",Sheet1!E91,"|",Sheet1!F91,"|",Sheet1!G91,"|",Sheet1!H91,"|",Sheet1!I91,"|",Sheet1!J91,"|",Sheet1!K91)</f>
         <v>extra_spearmint|02289902|1|Mars Inc Wrigley|Extra|Spearmint|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_spearmint.png</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="str">
+    <row r="91" spans="1:1">
+      <c r="A91" t="str">
         <f>CONCATENATE(Sheet1!A92,"|",Sheet1!B92,"|",Sheet1!C92,"|",Sheet1!D92,"|",Sheet1!E92,"|",Sheet1!F92,"|",Sheet1!G92,"|",Sheet1!H92,"|",Sheet1!I92,"|",Sheet1!J92,"|",Sheet1!K92)</f>
         <v>extra_peppermint|0|1|Mars Inc Wrigley|Extra|Peppermint|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_peppermint.png</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="str">
+    <row r="92" spans="1:1">
+      <c r="A92" t="str">
         <f>CONCATENATE(Sheet1!A93,"|",Sheet1!B93,"|",Sheet1!C93,"|",Sheet1!D93,"|",Sheet1!E93,"|",Sheet1!F93,"|",Sheet1!G93,"|",Sheet1!H93,"|",Sheet1!I93,"|",Sheet1!J93,"|",Sheet1!K93)</f>
         <v>extra_polar_ice|0|1|Mars Inc Wrigley|Extra|Polar Ice|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_polar_ice.png</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="str">
+    <row r="93" spans="1:1">
+      <c r="A93" t="str">
         <f>CONCATENATE(Sheet1!A94,"|",Sheet1!B94,"|",Sheet1!C94,"|",Sheet1!D94,"|",Sheet1!E94,"|",Sheet1!F94,"|",Sheet1!G94,"|",Sheet1!H94,"|",Sheet1!I94,"|",Sheet1!J94,"|",Sheet1!K94)</f>
         <v>extra_smooth_mint|0|1|Mars Inc Wrigley|Extra|Smooth Mint|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_smooth_mint.png</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="str">
+    <row r="94" spans="1:1">
+      <c r="A94" t="str">
         <f>CONCATENATE(Sheet1!A95,"|",Sheet1!B95,"|",Sheet1!C95,"|",Sheet1!D95,"|",Sheet1!E95,"|",Sheet1!F95,"|",Sheet1!G95,"|",Sheet1!H95,"|",Sheet1!I95,"|",Sheet1!J95,"|",Sheet1!K95)</f>
         <v>extra_winterfresh|02284004|1|Mars Inc Wrigley|Extra|Winterfresh|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_winterfresh.png</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="str">
+    <row r="95" spans="1:1">
+      <c r="A95" t="str">
         <f>CONCATENATE(Sheet1!A96,"|",Sheet1!B96,"|",Sheet1!C96,"|",Sheet1!D96,"|",Sheet1!E96,"|",Sheet1!F96,"|",Sheet1!G96,"|",Sheet1!H96,"|",Sheet1!I96,"|",Sheet1!J96,"|",Sheet1!K96)</f>
         <v>extra_classic_bubble|02284509|1|Mars Inc Wrigley|Extra|Classic Bubble|Launched in 1984, Extra was Wrigley's first sugar-free gum offering in the U.S. Extra gum is known for its incredible, long-lasting flavors. Extra gum is also available in a variety of distinctive flavors, specifically tailored to local tastes, in geographies including Australia, Canada, China, Germany, Hong Kong, New Zealand and Taiwan.||United States|0|extra_classic_bubble.png</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="str">
+    <row r="96" spans="1:1">
+      <c r="A96" t="str">
         <f>CONCATENATE(Sheet1!A97,"|",Sheet1!B97,"|",Sheet1!C97,"|",Sheet1!D97,"|",Sheet1!E97,"|",Sheet1!F97,"|",Sheet1!G97,"|",Sheet1!H97,"|",Sheet1!I97,"|",Sheet1!J97,"|",Sheet1!K97)</f>
-        <v>5_gum_rain|0|1|Mars Inc Wrigley|5 Gum|Rain|a tingling spearmint||United States|0|</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="str">
+        <v>5_gum_rain|0|1|Mars Inc Wrigley|5 Gum|Rain|a tingling spearmint||United States|0|5_gum_rain.jpg</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="str">
         <f>CONCATENATE(Sheet1!A98,"|",Sheet1!B98,"|",Sheet1!C98,"|",Sheet1!D98,"|",Sheet1!E98,"|",Sheet1!F98,"|",Sheet1!G98,"|",Sheet1!H98,"|",Sheet1!I98,"|",Sheet1!J98,"|",Sheet1!K98)</f>
-        <v>5_gum_cobalt|0|1|Mars Inc Wrigley|5 Gum|Cobalt|a cooling peppermint||United States|0|</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="str">
+        <v>5_gum_cobalt|0|1|Mars Inc Wrigley|5 Gum|Cobalt|a cooling peppermint||United States|0|5_gum_cobalt.jpg</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="str">
         <f>CONCATENATE(Sheet1!A99,"|",Sheet1!B99,"|",Sheet1!C99,"|",Sheet1!D99,"|",Sheet1!E99,"|",Sheet1!F99,"|",Sheet1!G99,"|",Sheet1!H99,"|",Sheet1!I99,"|",Sheet1!J99,"|",Sheet1!K99)</f>
-        <v>5_gum_flare|0|1|Mars Inc Wrigley|5 Gum|Flare|a warming cinnamon||United States|0|</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="str">
+        <v>5_gum_flare|0|1|Mars Inc Wrigley|5 Gum|Flare|a warming cinnamon||United States|0|5_gum_flare.jpg</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="str">
         <f>CONCATENATE(Sheet1!A100,"|",Sheet1!B100,"|",Sheet1!C100,"|",Sheet1!D100,"|",Sheet1!E100,"|",Sheet1!F100,"|",Sheet1!G100,"|",Sheet1!H100,"|",Sheet1!I100,"|",Sheet1!J100,"|",Sheet1!K100)</f>
-        <v>5_gum_elixir|0|1|Mars Inc Wrigley|5 Gum|Elixir|a mouthwatering berry||United States|0|</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="str">
+        <v>5_gum_elixir|0|1|Mars Inc Wrigley|5 Gum|Elixir|a mouthwatering berry||United States|0|5_gum_elixir.jpg</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="str">
         <f>CONCATENATE(Sheet1!A101,"|",Sheet1!B101,"|",Sheet1!C101,"|",Sheet1!D101,"|",Sheet1!E101,"|",Sheet1!F101,"|",Sheet1!G101,"|",Sheet1!H101,"|",Sheet1!I101,"|",Sheet1!J101,"|",Sheet1!K101)</f>
-        <v>5_gum_solstice|0|1|Mars Inc Wrigley|5 Gum|Solstice|a warm and cool winter||United States|0|</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="str">
+        <v>5_gum_solstice|0|1|Mars Inc Wrigley|5 Gum|Solstice|a warm and cool winter||United States|0|5_gum_solstice.jpg</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="str">
         <f>CONCATENATE(Sheet1!A102,"|",Sheet1!B102,"|",Sheet1!C102,"|",Sheet1!D102,"|",Sheet1!E102,"|",Sheet1!F102,"|",Sheet1!G102,"|",Sheet1!H102,"|",Sheet1!I102,"|",Sheet1!J102,"|",Sheet1!K102)</f>
-        <v>5_gum_react_fruit|022000116970|1|Mars Inc Wrigley|5 Gum|React Fruit|a unique fruit flavor experience||United States|0|</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="str">
+        <v>5_gum_react_fruit|022000116970|1|Mars Inc Wrigley|5 Gum|React Fruit|a unique fruit flavor experience||United States|0|5_gum_react_fruit.jpg</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="str">
         <f>CONCATENATE(Sheet1!A103,"|",Sheet1!B103,"|",Sheet1!C103,"|",Sheet1!D103,"|",Sheet1!E103,"|",Sheet1!F103,"|",Sheet1!G103,"|",Sheet1!H103,"|",Sheet1!I103,"|",Sheet1!J103,"|",Sheet1!K103)</f>
-        <v>5_gum_react_mint|022000117014|1|Mars Inc Wrigley|5 Gum|React Mint|a unique mint flavor experience||United States|0|</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="str">
+        <v>5_gum_react_mint|022000117014|1|Mars Inc Wrigley|5 Gum|React Mint|a unique mint flavor experience||United States|0|5_gum_react_mint.jpg</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="str">
         <f>CONCATENATE(Sheet1!A104,"|",Sheet1!B104,"|",Sheet1!C104,"|",Sheet1!D104,"|",Sheet1!E104,"|",Sheet1!F104,"|",Sheet1!G104,"|",Sheet1!H104,"|",Sheet1!I104,"|",Sheet1!J104,"|",Sheet1!K104)</f>
-        <v>5_gum_prism|0|1|Mars Inc Wrigley|5 Gum|Prism|an electric watermelon||United States|0|</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="str">
+        <v>5_gum_prism|0|1|Mars Inc Wrigley|5 Gum|Prism|an electric watermelon||United States|0|5_gum_prism.jpg</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="str">
         <f>CONCATENATE(Sheet1!A105,"|",Sheet1!B105,"|",Sheet1!C105,"|",Sheet1!D105,"|",Sheet1!E105,"|",Sheet1!F105,"|",Sheet1!G105,"|",Sheet1!H105,"|",Sheet1!I105,"|",Sheet1!J105,"|",Sheet1!K105)</f>
-        <v>5_gum_vortex|0|1|Mars Inc Wrigley|5 Gum|Vortex|a juicy green apple||United States|0|</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="str">
+        <v>5_gum_vortex|0|1|Mars Inc Wrigley|5 Gum|Vortex|a juicy green apple||United States|0|5_gum_vortex.jpg</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="str">
         <f>CONCATENATE(Sheet1!A106,"|",Sheet1!B106,"|",Sheet1!C106,"|",Sheet1!D106,"|",Sheet1!E106,"|",Sheet1!F106,"|",Sheet1!G106,"|",Sheet1!H106,"|",Sheet1!I106,"|",Sheet1!J106,"|",Sheet1!K106)</f>
-        <v>5_gum_swerve|022000013170|1|Mars Inc Wrigley|5 Gum|Swerve|a tangy to sweet tropical||United States|0|</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="str">
+        <v>5_gum_swerve|022000013170|1|Mars Inc Wrigley|5 Gum|Swerve|a tangy to sweet tropical||United States|0|5_gum_swerve.jpg</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="str">
         <f>CONCATENATE(Sheet1!A107,"|",Sheet1!B107,"|",Sheet1!C107,"|",Sheet1!D107,"|",Sheet1!E107,"|",Sheet1!F107,"|",Sheet1!G107,"|",Sheet1!H107,"|",Sheet1!I107,"|",Sheet1!J107,"|",Sheet1!K107)</f>
-        <v>5_gum_rpm_fruit|0|1|Mars Inc Wrigley|5 Gum|RPM Fruit|an energizing fruit flavor||United States|0|</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="str">
+        <v>5_gum_rpm_fruit|0|1|Mars Inc Wrigley|5 Gum|RPM Fruit|an energizing fruit flavor||United States|0|5_gum_rpm_fruit.jpg</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="str">
         <f>CONCATENATE(Sheet1!A108,"|",Sheet1!B108,"|",Sheet1!C108,"|",Sheet1!D108,"|",Sheet1!E108,"|",Sheet1!F108,"|",Sheet1!G108,"|",Sheet1!H108,"|",Sheet1!I108,"|",Sheet1!J108,"|",Sheet1!K108)</f>
-        <v>5_gum_rpm_mint|0|1|Mars Inc Wrigley|5 Gum|RPM Mint|a relaxing mint flavor||United States|0|</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="str">
+        <v>5_gum_rpm_mint|0|1|Mars Inc Wrigley|5 Gum|RPM Mint|a relaxing mint flavor||United States|0|5_gum_rpm_mint.jpg</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="str">
         <f>CONCATENATE(Sheet1!A109,"|",Sheet1!B109,"|",Sheet1!C109,"|",Sheet1!D109,"|",Sheet1!E109,"|",Sheet1!F109,"|",Sheet1!G109,"|",Sheet1!H109,"|",Sheet1!I109,"|",Sheet1!J109,"|",Sheet1!K109)</f>
         <v>wrigleys_big_red_cinnamon|0|1|Mars Inc Wrigley|Wrigley's Big Red|Cinnamon|?||United States|0|wrigleys_big_red_cinnamon.jpg</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="str">
+    <row r="109" spans="1:1">
+      <c r="A109" t="str">
         <f>CONCATENATE(Sheet1!A110,"|",Sheet1!B110,"|",Sheet1!C110,"|",Sheet1!D110,"|",Sheet1!E110,"|",Sheet1!F110,"|",Sheet1!G110,"|",Sheet1!H110,"|",Sheet1!I110,"|",Sheet1!J110,"|",Sheet1!K110)</f>
         <v>wrigleys_doublemint_mint|0|1|Mars Inc Wrigley|Wrigley's Doublemint|Mint|?||United States|0|wrigleys_doublemint_mint.jpg</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="str">
+    <row r="110" spans="1:1">
+      <c r="A110" t="str">
         <f>CONCATENATE(Sheet1!A111,"|",Sheet1!B111,"|",Sheet1!C111,"|",Sheet1!D111,"|",Sheet1!E111,"|",Sheet1!F111,"|",Sheet1!G111,"|",Sheet1!H111,"|",Sheet1!I111,"|",Sheet1!J111,"|",Sheet1!K111)</f>
         <v>eclipse_spearmint|0|1|Mars Inc Wrigley|Eclipse|Spearmint|?||United States|0|eclipse_spearmint.jpg</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="str">
+    <row r="111" spans="1:1">
+      <c r="A111" t="str">
         <f>CONCATENATE(Sheet1!A112,"|",Sheet1!B112,"|",Sheet1!C112,"|",Sheet1!D112,"|",Sheet1!E112,"|",Sheet1!F112,"|",Sheet1!G112,"|",Sheet1!H112,"|",Sheet1!I112,"|",Sheet1!J112,"|",Sheet1!K112)</f>
         <v>eclipse_polar_ice|0|1|Mars Inc Wrigley|Eclipse|Polar Ice|?||United States|0|eclipse_polar_ice.jpg</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="str">
+    <row r="112" spans="1:1">
+      <c r="A112" t="str">
         <f>CONCATENATE(Sheet1!A113,"|",Sheet1!B113,"|",Sheet1!C113,"|",Sheet1!D113,"|",Sheet1!E113,"|",Sheet1!F113,"|",Sheet1!G113,"|",Sheet1!H113,"|",Sheet1!I113,"|",Sheet1!J113,"|",Sheet1!K113)</f>
         <v>eclipse_peppermint|0|1|Mars Inc Wrigley|Eclipse|Peppermint|?||United States|0|eclipse_peppermint.jpg</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="str">
+    <row r="113" spans="1:1">
+      <c r="A113" t="str">
         <f>CONCATENATE(Sheet1!A114,"|",Sheet1!B114,"|",Sheet1!C114,"|",Sheet1!D114,"|",Sheet1!E114,"|",Sheet1!F114,"|",Sheet1!G114,"|",Sheet1!H114,"|",Sheet1!I114,"|",Sheet1!J114,"|",Sheet1!K114)</f>
         <v>eclipse_winterfrost|0|1|Mars Inc Wrigley|Eclipse|Winterfrost|?||United States|0|eclipse_winterfrost.jpg</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="str">
+    <row r="114" spans="1:1">
+      <c r="A114" t="str">
         <f>CONCATENATE(Sheet1!A115,"|",Sheet1!B115,"|",Sheet1!C115,"|",Sheet1!D115,"|",Sheet1!E115,"|",Sheet1!F115,"|",Sheet1!G115,"|",Sheet1!H115,"|",Sheet1!I115,"|",Sheet1!J115,"|",Sheet1!K115)</f>
         <v>freedent_peppermint|0|1|Mars Inc Wrigley|Freedent|Peppermint|?||United States|0|freedent_peppermint.jpg</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="str">
+    <row r="115" spans="1:1">
+      <c r="A115" t="str">
         <f>CONCATENATE(Sheet1!A116,"|",Sheet1!B116,"|",Sheet1!C116,"|",Sheet1!D116,"|",Sheet1!E116,"|",Sheet1!F116,"|",Sheet1!G116,"|",Sheet1!H116,"|",Sheet1!I116,"|",Sheet1!J116,"|",Sheet1!K116)</f>
         <v>freedent_spearmint|0|1|Mars Inc Wrigley|Freedent|Spearmint|?||United States|0|freedent_spearmint.jpg</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="str">
+    <row r="116" spans="1:1">
+      <c r="A116" t="str">
         <f>CONCATENATE(Sheet1!A117,"|",Sheet1!B117,"|",Sheet1!C117,"|",Sheet1!D117,"|",Sheet1!E117,"|",Sheet1!F117,"|",Sheet1!G117,"|",Sheet1!H117,"|",Sheet1!I117,"|",Sheet1!J117,"|",Sheet1!K117)</f>
         <v>freedent_winterfresh|0|1|Mars Inc Wrigley|Freedent|Winterfresh|?||United States|0|freedent_winterfresh.jpg</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="str">
+    <row r="117" spans="1:1">
+      <c r="A117" t="str">
         <f>CONCATENATE(Sheet1!A118,"|",Sheet1!B118,"|",Sheet1!C118,"|",Sheet1!D118,"|",Sheet1!E118,"|",Sheet1!F118,"|",Sheet1!G118,"|",Sheet1!H118,"|",Sheet1!I118,"|",Sheet1!J118,"|",Sheet1!K118)</f>
         <v>hubba_bubba_max_outrageous_original|0|1|Mars Inc Wrigley|Hubba Bubba Max|Outrageous Original|||United States|0|</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="str">
+    <row r="118" spans="1:1">
+      <c r="A118" t="str">
         <f>CONCATENATE(Sheet1!A119,"|",Sheet1!B119,"|",Sheet1!C119,"|",Sheet1!D119,"|",Sheet1!E119,"|",Sheet1!F119,"|",Sheet1!G119,"|",Sheet1!H119,"|",Sheet1!I119,"|",Sheet1!J119,"|",Sheet1!K119)</f>
         <v>hubba_bubba_max_strawberry_watermelon|0|1|Mars Inc Wrigley|Hubba Bubba Max|Strawberry Watermelon|||United States|0|</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="str">
+    <row r="119" spans="1:1">
+      <c r="A119" t="str">
         <f>CONCATENATE(Sheet1!A120,"|",Sheet1!B120,"|",Sheet1!C120,"|",Sheet1!D120,"|",Sheet1!E120,"|",Sheet1!F120,"|",Sheet1!G120,"|",Sheet1!H120,"|",Sheet1!I120,"|",Sheet1!J120,"|",Sheet1!K120)</f>
         <v>hubba_bubba_max_sweet_&amp;_sassy_cherry|0|1|Mars Inc Wrigley|Hubba Bubba Max|Sweet &amp; Sassy Cherry|||United States|0|</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="str">
+    <row r="120" spans="1:1">
+      <c r="A120" t="str">
         <f>CONCATENATE(Sheet1!A121,"|",Sheet1!B121,"|",Sheet1!C121,"|",Sheet1!D121,"|",Sheet1!E121,"|",Sheet1!F121,"|",Sheet1!G121,"|",Sheet1!H121,"|",Sheet1!I121,"|",Sheet1!J121,"|",Sheet1!K121)</f>
         <v>hubba_bubba_max_mystery_flavor|0|1|Mars Inc Wrigley|Hubba Bubba Max|Mystery Flavor|||United States|0|</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="str">
+    <row r="121" spans="1:1">
+      <c r="A121" t="str">
         <f>CONCATENATE(Sheet1!A122,"|",Sheet1!B122,"|",Sheet1!C122,"|",Sheet1!D122,"|",Sheet1!E122,"|",Sheet1!F122,"|",Sheet1!G122,"|",Sheet1!H122,"|",Sheet1!I122,"|",Sheet1!J122,"|",Sheet1!K122)</f>
         <v>hubba_bubba_squeeze_pop_assorted_sour_flavors|0|1|Mars Inc Wrigley|Hubba Bubba Squeeze Pop|Assorted Sour Flavors|||United States|0|</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="str">
+    <row r="122" spans="1:1">
+      <c r="A122" t="str">
         <f>CONCATENATE(Sheet1!A123,"|",Sheet1!B123,"|",Sheet1!C123,"|",Sheet1!D123,"|",Sheet1!E123,"|",Sheet1!F123,"|",Sheet1!G123,"|",Sheet1!H123,"|",Sheet1!I123,"|",Sheet1!J123,"|",Sheet1!K123)</f>
         <v>hubba_bubba_bubble_tape_awesome_original|0|1|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Awesome Original|||United States|0|</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="str">
+    <row r="123" spans="1:1">
+      <c r="A123" t="str">
         <f>CONCATENATE(Sheet1!A124,"|",Sheet1!B124,"|",Sheet1!C124,"|",Sheet1!D124,"|",Sheet1!E124,"|",Sheet1!F124,"|",Sheet1!G124,"|",Sheet1!H124,"|",Sheet1!I124,"|",Sheet1!J124,"|",Sheet1!K124)</f>
         <v>hubba_bubba_bubble_tape_snappy_strawberry|0|1|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Snappy Strawberry|||United States|0|</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="str">
+    <row r="124" spans="1:1">
+      <c r="A124" t="str">
         <f>CONCATENATE(Sheet1!A125,"|",Sheet1!B125,"|",Sheet1!C125,"|",Sheet1!D125,"|",Sheet1!E125,"|",Sheet1!F125,"|",Sheet1!G125,"|",Sheet1!H125,"|",Sheet1!I125,"|",Sheet1!J125,"|",Sheet1!K125)</f>
         <v>hubba_bubba_bubble_tape_sour_apple|0|1|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Sour Apple|||United States|0|</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
-      <c r="A110" t="str">
+    <row r="125" spans="1:1">
+      <c r="A125" t="str">
         <f>CONCATENATE(Sheet1!A126,"|",Sheet1!B126,"|",Sheet1!C126,"|",Sheet1!D126,"|",Sheet1!E126,"|",Sheet1!F126,"|",Sheet1!G126,"|",Sheet1!H126,"|",Sheet1!I126,"|",Sheet1!J126,"|",Sheet1!K126)</f>
         <v>hubba_bubba_bubble_tape_triple_treat|0|1|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Triple Treat|||United States|0|</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="str">
+    <row r="126" spans="1:1">
+      <c r="A126" t="str">
         <f>CONCATENATE(Sheet1!A127,"|",Sheet1!B127,"|",Sheet1!C127,"|",Sheet1!D127,"|",Sheet1!E127,"|",Sheet1!F127,"|",Sheet1!G127,"|",Sheet1!H127,"|",Sheet1!I127,"|",Sheet1!J127,"|",Sheet1!K127)</f>
         <v>hubba_bubba_bubble_tape_tangy_tropical|0|1|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Tangy Tropical|||United States|0|</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
-      <c r="A112" t="str">
+    <row r="127" spans="1:1">
+      <c r="A127" t="str">
         <f>CONCATENATE(Sheet1!A128,"|",Sheet1!B128,"|",Sheet1!C128,"|",Sheet1!D128,"|",Sheet1!E128,"|",Sheet1!F128,"|",Sheet1!G128,"|",Sheet1!H128,"|",Sheet1!I128,"|",Sheet1!J128,"|",Sheet1!K128)</f>
         <v>hubba_bubba_bubble_tape_mystery_flavor|0|1|Mars Inc Wrigley|Hubba Bubba Bubble Tape|Mystery Flavor|||United States|0|</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="str">
+    <row r="128" spans="1:1">
+      <c r="A128" t="str">
         <f>CONCATENATE(Sheet1!A129,"|",Sheet1!B129,"|",Sheet1!C129,"|",Sheet1!D129,"|",Sheet1!E129,"|",Sheet1!F129,"|",Sheet1!G129,"|",Sheet1!H129,"|",Sheet1!I129,"|",Sheet1!J129,"|",Sheet1!K129)</f>
         <v>hubba_bubba_ouch!_bubble_gum|0|1|Mars Inc Wrigley|Hubba Bubba OUCH!|Bubble Gum|||United States|0|</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="str">
+    <row r="129" spans="1:1">
+      <c r="A129" t="str">
         <f>CONCATENATE(Sheet1!A130,"|",Sheet1!B130,"|",Sheet1!C130,"|",Sheet1!D130,"|",Sheet1!E130,"|",Sheet1!F130,"|",Sheet1!G130,"|",Sheet1!H130,"|",Sheet1!I130,"|",Sheet1!J130,"|",Sheet1!K130)</f>
         <v>wrigleys_juicy_fruit_juicy_secret|0|1|Mars Inc Wrigley|Wrigley's Juicy Fruit|Juicy Secret|||United States|0|</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
-      <c r="A115" t="str">
+    <row r="130" spans="1:1">
+      <c r="A130" t="str">
         <f>CONCATENATE(Sheet1!A131,"|",Sheet1!B131,"|",Sheet1!C131,"|",Sheet1!D131,"|",Sheet1!E131,"|",Sheet1!F131,"|",Sheet1!G131,"|",Sheet1!H131,"|",Sheet1!I131,"|",Sheet1!J131,"|",Sheet1!K131)</f>
         <v>wrigleys_juicy_fruit_original|0|1|Mars Inc Wrigley|Wrigley's Juicy Fruit|Original|||United States|0|</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="str">
+    <row r="131" spans="1:1">
+      <c r="A131" t="str">
         <f>CONCATENATE(Sheet1!A132,"|",Sheet1!B132,"|",Sheet1!C132,"|",Sheet1!D132,"|",Sheet1!E132,"|",Sheet1!F132,"|",Sheet1!G132,"|",Sheet1!H132,"|",Sheet1!I132,"|",Sheet1!J132,"|",Sheet1!K132)</f>
         <v>wrigleys_juicy_fruit_sweet_fruit|0|1|Mars Inc Wrigley|Wrigley's Juicy Fruit|Sweet Fruit|||United States|0|</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
-      <c r="A117" t="str">
+    <row r="132" spans="1:1">
+      <c r="A132" t="str">
         <f>CONCATENATE(Sheet1!A133,"|",Sheet1!B133,"|",Sheet1!C133,"|",Sheet1!D133,"|",Sheet1!E133,"|",Sheet1!F133,"|",Sheet1!G133,"|",Sheet1!H133,"|",Sheet1!I133,"|",Sheet1!J133,"|",Sheet1!K133)</f>
         <v>wrigleys_juicy_fruit_sweet_berry|0|1|Mars Inc Wrigley|Wrigley's Juicy Fruit|Sweet Berry|||United States|0|</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
-      <c r="A118" t="str">
+    <row r="133" spans="1:1">
+      <c r="A133" t="str">
         <f>CONCATENATE(Sheet1!A134,"|",Sheet1!B134,"|",Sheet1!C134,"|",Sheet1!D134,"|",Sheet1!E134,"|",Sheet1!F134,"|",Sheet1!G134,"|",Sheet1!H134,"|",Sheet1!I134,"|",Sheet1!J134,"|",Sheet1!K134)</f>
         <v>wrigleys_juicy_fruit_groovy_fruity|0|1|Mars Inc Wrigley|Wrigley's Juicy Fruit|Groovy Fruity|||United States|0|</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119" t="str">
-        <f>CONCATENATE(Sheet1!A135,"|",Sheet1!B135,"|",Sheet1!C135,"|",Sheet1!D135,"|",Sheet1!E135,"|",Sheet1!F135,"|",Sheet1!G135,"|",Sheet1!H135,"|",Sheet1!I135,"|",Sheet1!J135,"|",Sheet1!K135)</f>
-        <v>orbit_peppermint|0|1|Mars Inc Wrigley|Orbit|Peppermint|||United States|0|</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="str">
-        <f>CONCATENATE(Sheet1!A136,"|",Sheet1!B136,"|",Sheet1!C136,"|",Sheet1!D136,"|",Sheet1!E136,"|",Sheet1!F136,"|",Sheet1!G136,"|",Sheet1!H136,"|",Sheet1!I136,"|",Sheet1!J136,"|",Sheet1!K136)</f>
-        <v>orbit_spearmint|022000013958|1|Mars Inc Wrigley|Orbit|Spearmint|||United States|0|</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" t="str">
-        <f>CONCATENATE(Sheet1!A137,"|",Sheet1!B137,"|",Sheet1!C137,"|",Sheet1!D137,"|",Sheet1!E137,"|",Sheet1!F137,"|",Sheet1!G137,"|",Sheet1!H137,"|",Sheet1!I137,"|",Sheet1!J137,"|",Sheet1!K137)</f>
-        <v>orbit_bubblemint|0|1|Mars Inc Wrigley|Orbit|Bubblemint|||United States|0|</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
-      <c r="A122" t="str">
-        <f>CONCATENATE(Sheet1!A138,"|",Sheet1!B138,"|",Sheet1!C138,"|",Sheet1!D138,"|",Sheet1!E138,"|",Sheet1!F138,"|",Sheet1!G138,"|",Sheet1!H138,"|",Sheet1!I138,"|",Sheet1!J138,"|",Sheet1!K138)</f>
-        <v>orbit_wintermint|0|1|Mars Inc Wrigley|Orbit|Wintermint|||United States|0|</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123" t="str">
-        <f>CONCATENATE(Sheet1!A139,"|",Sheet1!B139,"|",Sheet1!C139,"|",Sheet1!D139,"|",Sheet1!E139,"|",Sheet1!F139,"|",Sheet1!G139,"|",Sheet1!H139,"|",Sheet1!I139,"|",Sheet1!J139,"|",Sheet1!K139)</f>
-        <v>orbit_cinnamint|0|1|Mars Inc Wrigley|Orbit|Cinnamint|||United States|0|</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1">
-      <c r="A124" t="str">
-        <f>CONCATENATE(Sheet1!A140,"|",Sheet1!B140,"|",Sheet1!C140,"|",Sheet1!D140,"|",Sheet1!E140,"|",Sheet1!F140,"|",Sheet1!G140,"|",Sheet1!H140,"|",Sheet1!I140,"|",Sheet1!J140,"|",Sheet1!K140)</f>
-        <v>orbit_sweetmint|0|1|Mars Inc Wrigley|Orbit|Sweetmint|||United States|0|</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1">
-      <c r="A125" t="str">
-        <f>CONCATENATE(Sheet1!A141,"|",Sheet1!B141,"|",Sheet1!C141,"|",Sheet1!D141,"|",Sheet1!E141,"|",Sheet1!F141,"|",Sheet1!G141,"|",Sheet1!H141,"|",Sheet1!I141,"|",Sheet1!J141,"|",Sheet1!K141)</f>
-        <v>orbit_maui_melon_mint|0|1|Mars Inc Wrigley|Orbit|Maui Melon Mint|||United States|0|</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126" t="str">
-        <f>CONCATENATE(Sheet1!A142,"|",Sheet1!B142,"|",Sheet1!C142,"|",Sheet1!D142,"|",Sheet1!E142,"|",Sheet1!F142,"|",Sheet1!G142,"|",Sheet1!H142,"|",Sheet1!I142,"|",Sheet1!J142,"|",Sheet1!K142)</f>
-        <v>orbit_wildberry_remix|0|1|Mars Inc Wrigley|Orbit|Wildberry Remix|||United States|0|</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="str">
-        <f>CONCATENATE(Sheet1!A143,"|",Sheet1!B143,"|",Sheet1!C143,"|",Sheet1!D143,"|",Sheet1!E143,"|",Sheet1!F143,"|",Sheet1!G143,"|",Sheet1!H143,"|",Sheet1!I143,"|",Sheet1!J143,"|",Sheet1!K143)</f>
-        <v>orbit_melon_remix|0|1|Mars Inc Wrigley|Orbit|Melon Remix|||United States|0|</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" t="str">
-        <f>CONCATENATE(Sheet1!A144,"|",Sheet1!B144,"|",Sheet1!C144,"|",Sheet1!D144,"|",Sheet1!E144,"|",Sheet1!F144,"|",Sheet1!G144,"|",Sheet1!H144,"|",Sheet1!I144,"|",Sheet1!J144,"|",Sheet1!K144)</f>
-        <v>orbit_tropical_remix|0|1|Mars Inc Wrigley|Orbit|Tropical Remix|||United States|0|</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129" t="str">
-        <f>CONCATENATE(Sheet1!A145,"|",Sheet1!B145,"|",Sheet1!C145,"|",Sheet1!D145,"|",Sheet1!E145,"|",Sheet1!F145,"|",Sheet1!G145,"|",Sheet1!H145,"|",Sheet1!I145,"|",Sheet1!J145,"|",Sheet1!K145)</f>
-        <v>orbit_strawberry_remix|0|1|Mars Inc Wrigley|Orbit|Strawberry Remix|||United States|0|</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
-      <c r="A130" t="str">
-        <f>CONCATENATE(Sheet1!A146,"|",Sheet1!B146,"|",Sheet1!C146,"|",Sheet1!D146,"|",Sheet1!E146,"|",Sheet1!F146,"|",Sheet1!G146,"|",Sheet1!H146,"|",Sheet1!I146,"|",Sheet1!J146,"|",Sheet1!K146)</f>
-        <v>orbit_mist_raspberry_lemon_dew|0|1|Mars Inc Wrigley|Orbit Mist|Raspberry Lemon Dew|||United States|0|</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131" t="str">
-        <f>CONCATENATE(Sheet1!A147,"|",Sheet1!B147,"|",Sheet1!C147,"|",Sheet1!D147,"|",Sheet1!E147,"|",Sheet1!F147,"|",Sheet1!G147,"|",Sheet1!H147,"|",Sheet1!I147,"|",Sheet1!J147,"|",Sheet1!K147)</f>
-        <v>orbit_mist_peppermint_spray|0|1|Mars Inc Wrigley|Orbit Mist|Peppermint Spray|||United States|0|</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" t="str">
-        <f>CONCATENATE(Sheet1!A148,"|",Sheet1!B148,"|",Sheet1!C148,"|",Sheet1!D148,"|",Sheet1!E148,"|",Sheet1!F148,"|",Sheet1!G148,"|",Sheet1!H148,"|",Sheet1!I148,"|",Sheet1!J148,"|",Sheet1!K148)</f>
-        <v>orbit_mist_spearmint_spritzer|0|1|Mars Inc Wrigley|Orbit Mist|Spearmint Spritzer|||United States|0|</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133" t="str">
-        <f>CONCATENATE(Sheet1!A149,"|",Sheet1!B149,"|",Sheet1!C149,"|",Sheet1!D149,"|",Sheet1!E149,"|",Sheet1!F149,"|",Sheet1!G149,"|",Sheet1!H149,"|",Sheet1!I149,"|",Sheet1!J149,"|",Sheet1!K149)</f>
-        <v>orbit_mist_watermelon_spring|0|1|Mars Inc Wrigley|Orbit Mist|Watermelon Spring|||United States|0|</v>
       </c>
     </row>
   </sheetData>

</xml_diff>